<commit_message>
Update DR# 622 Journeytech Inc. (KO Ribbons)_10_23_2020.xlsx
</commit_message>
<xml_diff>
--- a/DR# 622 Journeytech Inc. (KO Ribbons)_10_23_2020.xlsx
+++ b/DR# 622 Journeytech Inc. (KO Ribbons)_10_23_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B40B7B4-51A2-41FB-8654-DF96D4E88656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DB9DE4-02F0-44B8-B265-32126D91F6D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1372,7 +1372,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1499,10 +1499,10 @@
         <v>28</v>
       </c>
       <c r="C15" s="35">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D15" s="35">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E15" s="39" t="s">
         <v>29</v>

</xml_diff>